<commit_message>
Committing DTS400 Materials including final version of rmd.  11:20 24Nov
</commit_message>
<xml_diff>
--- a/DTS350TemplateMaster/DTS400/Code Review.xlsx
+++ b/DTS350TemplateMaster/DTS400/Code Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\000 DTS 350 Data Visualization\DTS350-hollinbergert\DTS350TemplateMaster\DTS400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90CC7CAC-C819-4BD0-B518-C28CB6D9A78E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C19B6C3-97B9-4663-8381-8F82FF68ADA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="930" windowWidth="24240" windowHeight="13140" xr2:uid="{CA2721B9-F12A-4149-A4A4-51139866A922}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="133">
   <si>
     <t>check Workfile 3 vs workfile3a  &gt;&gt; rename best to workfile3</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>Good Plots</t>
-  </si>
-  <si>
-    <t>GE Plots of continuous vars</t>
-  </si>
-  <si>
-    <t>GE Plots of continuous vars2</t>
   </si>
   <si>
     <t>Workfile2</t>
@@ -309,9 +303,6 @@
     <t>wgpa x extyn (exit)            saved to PLOTS</t>
   </si>
   <si>
-    <t>change x axis label on wgpa x exit  GE2 2115</t>
-  </si>
-  <si>
     <t>wgpa x rnk</t>
   </si>
   <si>
@@ -343,13 +334,181 @@
   </si>
   <si>
     <t>wgpa x dst</t>
+  </si>
+  <si>
+    <t>GE2 Plots of continuous vars</t>
+  </si>
+  <si>
+    <t>GE2 Plots of continuous vars2</t>
+  </si>
+  <si>
+    <t>GE3 Linear Regressions</t>
+  </si>
+  <si>
+    <t>Gewfb</t>
+  </si>
+  <si>
+    <t>Read-In GWwfb worksheet</t>
+  </si>
+  <si>
+    <t>Set GE3 Linear Regression as working file</t>
+  </si>
+  <si>
+    <t>Full-Up Correlation Plot red and blue ellipses  saved to corrplotalllevels.jpeg</t>
+  </si>
+  <si>
+    <t>narrow the list of variables corrplot ellipses</t>
+  </si>
+  <si>
+    <t>corrplot w/ wgpa, rnkneg, tcr, hsgpa,	cmp,	mat,	sci,	eng,	rdg)</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
+  </si>
+  <si>
+    <t>ScatterplotMatrix shows distribution of each variable, and correlation plot for all pairs</t>
+  </si>
+  <si>
+    <t>ScatterplotMatrix of wgpa, rnkneg, hsgpa, tcr, eng, rdg)</t>
+  </si>
+  <si>
+    <t>Regress hsgpa with wgpa and plot diagnostics 4-panel</t>
+  </si>
+  <si>
+    <t>diagnosticplot_hsg_rnkneg_eng_mat</t>
+  </si>
+  <si>
+    <t>Look at outliers  -- use their numeric order number</t>
+  </si>
+  <si>
+    <t>All In MLR AdjRsqd .4322</t>
+  </si>
+  <si>
+    <t>All In MLR 4 panel diagnostic</t>
+  </si>
+  <si>
+    <t>All In MLR AdjRsqd .469  GRADS ONLY</t>
+  </si>
+  <si>
+    <t>Standardize all variables</t>
+  </si>
+  <si>
+    <t>All In Standardized MLR AdjRsqd .4322</t>
+  </si>
+  <si>
+    <t>All In Standardized MLR AdjRsqd GRADS ONLY .469</t>
+  </si>
+  <si>
+    <t>TopHalfIVs .4412</t>
+  </si>
+  <si>
+    <t>StatSig Ivs   rnkneg + gndr + hst3 + mat + dst + hsgpa + rdg    .438</t>
+  </si>
+  <si>
+    <t>wgpa ~ rnk + gndr + hst3 + mat + dst + hsgpa</t>
+  </si>
+  <si>
+    <t>plot_summ of est coeffs   hsgpa + dst + mat + hst3 + gndr + rnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnostic plots 4 panel </t>
+  </si>
+  <si>
+    <t>Classic Ivs  wgpa ~ rnk + hsgpa + mat + eng + rdg + cmp + sci + tcr    .3894</t>
+  </si>
+  <si>
+    <t>plot_summ of est coeffs   tcr + sci + cmp + rdg + eng + mat + hsgpa + rnk</t>
+  </si>
+  <si>
+    <t>plot_sum both on same graph statsig and classic</t>
+  </si>
+  <si>
+    <t>diagnostic plot 4 panel Classic Ivs</t>
+  </si>
+  <si>
+    <t>Standardized Classiv Ivs  .384</t>
+  </si>
+  <si>
+    <t>plot_summ without bellcurves</t>
+  </si>
+  <si>
+    <t>diagnostic plot 4 panel Classic Ivs Standardized</t>
+  </si>
+  <si>
+    <t>Only Statistically Significant IVs  Pr &lt;.05  using standardized continuous variables wgpa ~ rnkneg + gndr + hst3 + mat + dst + hsgpa + rdg,   .438</t>
+  </si>
+  <si>
+    <t>Plot-Summ with bellcurves and Grad, Exit, Both using classic Ivs</t>
+  </si>
+  <si>
+    <t>gvlma  Assessment of Linear Regression Model Assumptions</t>
+  </si>
+  <si>
+    <t>GE4 Probit</t>
+  </si>
+  <si>
+    <t>Readin Workfile3 and Gwwofb</t>
+  </si>
+  <si>
+    <t>Pink and Blue Stacked Dots  #PLOT a HISTOGRAM OF GRADES</t>
+  </si>
+  <si>
+    <t>Probit all-in Ivs AIC = 60</t>
+  </si>
+  <si>
+    <t>Probit 11 best pvalues  AIC = 64</t>
+  </si>
+  <si>
+    <t>Run a set if single IVs and track on a excel spreadsheet PROBIT SINGLE IVs MODEL RUNS, in the ORIG LIST folder</t>
+  </si>
+  <si>
+    <t>Probit ext ~yr    AIC = 127.81</t>
+  </si>
+  <si>
+    <t>Probit Using Statistically Sig (P&lt;.10) from the Single IV Models      ext ~ wgpa + prnk + hsgpa + rnk + tcr + mat + yr + race5 + gndr  AIC = 63.68</t>
+  </si>
+  <si>
+    <t>Run Using Statistically Sig (P&lt;.05) from the Single IV Models    ext ~ wgpa + prnk + hsgpa + rnk + tcr + mat     AIC = 59.743</t>
+  </si>
+  <si>
+    <t>With rank,not prnk    ext ~ wgpa + hsgpa + rnk + tcr + mat    AIC = 58.286</t>
+  </si>
+  <si>
+    <t>ext ~ wgpa + prnk + hsgpa + tcr    AIC = 61.724</t>
+  </si>
+  <si>
+    <t>ext ~ wgpa + prnk + hsgpa + mat   AIC = 63.64</t>
+  </si>
+  <si>
+    <t>IMPORTANT FORK to Excel for Real-Statistics 2x2 Grid     "WORKFILE3 / PROBIT 1 using RS"  using wgpa,prnk,hsgpa,tcr,mat</t>
+  </si>
+  <si>
+    <t>IMPORTANT FORK to Excel for Real-Statistics 2x2 Grid     "WORKFILE3 / PROBIT 2 using RS"  using prnk,hsgpa,tcr,mat   since wgpa isn't known well in advance</t>
+  </si>
+  <si>
+    <t>BEST COMBINATION :   ext ~ wgpa + prnk + hsgpa + tcr + mat     AIC 57.797, BEST</t>
+  </si>
+  <si>
+    <t>Throw out WGPA since it is not well-known in advance  AIC = 72.584 : Lose a lot by throwing out wgpa</t>
+  </si>
+  <si>
+    <t>BEST MODEL With prnk not rank ext ~ wgpa + prnk + hsgpa + tcr + mat   AIC = 57.797</t>
+  </si>
+  <si>
+    <t>Regressions with Midband</t>
+  </si>
+  <si>
+    <t>Make the midband wgpa between 2.3 and 3.3</t>
+  </si>
+  <si>
+    <t>change x axis label on wgpa x exit  GE2 1833</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +520,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -386,8 +551,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF6F92E-CD2A-412B-B761-E82C01F33C34}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="N71" sqref="N71"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1084,401 +1250,1681 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s">
-        <v>39</v>
-      </c>
       <c r="F34" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E36">
         <v>33</v>
       </c>
       <c r="F36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
       <c r="E37">
         <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
       <c r="E38">
         <v>47</v>
       </c>
       <c r="F38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
+      </c>
       <c r="E39">
         <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>40</v>
+      </c>
       <c r="E40">
         <v>87</v>
       </c>
       <c r="F40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
       <c r="E41">
         <v>96</v>
       </c>
       <c r="F41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
       <c r="E42">
         <v>98</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>40</v>
+      </c>
       <c r="E43">
         <v>109</v>
       </c>
       <c r="F43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
       <c r="E44">
         <v>120</v>
       </c>
       <c r="F44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" t="s">
+        <v>40</v>
+      </c>
       <c r="E45">
         <v>128</v>
       </c>
       <c r="F45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" t="s">
+        <v>40</v>
+      </c>
       <c r="E46">
         <v>133</v>
       </c>
       <c r="F46" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
       <c r="E47">
         <v>163</v>
       </c>
       <c r="F47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" t="s">
+        <v>40</v>
+      </c>
       <c r="E48">
         <v>186</v>
       </c>
       <c r="F48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
+        <v>40</v>
+      </c>
       <c r="E49">
         <v>186</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>40</v>
+      </c>
       <c r="E50">
         <v>282</v>
       </c>
       <c r="F50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>40</v>
+      </c>
       <c r="E51">
         <v>186</v>
       </c>
       <c r="F51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>40</v>
+      </c>
       <c r="E52">
         <v>286</v>
       </c>
       <c r="F52" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" t="s">
+        <v>40</v>
+      </c>
       <c r="E53">
         <v>386</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" t="s">
+        <v>40</v>
+      </c>
       <c r="E54">
         <v>486</v>
       </c>
       <c r="F54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" t="s">
+        <v>40</v>
+      </c>
       <c r="E55">
         <v>586</v>
       </c>
       <c r="F55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" t="s">
+        <v>40</v>
+      </c>
       <c r="E56">
         <v>686</v>
       </c>
       <c r="F56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
       <c r="E57">
         <v>786</v>
       </c>
       <c r="F57" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" t="s">
+        <v>40</v>
+      </c>
       <c r="E58">
         <v>886</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" t="s">
+        <v>40</v>
+      </c>
       <c r="E59">
         <v>986</v>
       </c>
       <c r="F59" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" t="s">
+        <v>40</v>
+      </c>
       <c r="E60">
         <v>1086</v>
       </c>
       <c r="F60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" t="s">
+        <v>40</v>
+      </c>
       <c r="E61">
         <v>1186</v>
       </c>
       <c r="F61" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" t="s">
+        <v>40</v>
+      </c>
       <c r="E62">
         <v>1286</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" t="s">
+        <v>40</v>
+      </c>
       <c r="E63">
         <v>1389</v>
       </c>
       <c r="F63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" t="s">
+        <v>40</v>
+      </c>
       <c r="E64">
         <v>1399</v>
       </c>
       <c r="F64" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" t="s">
+        <v>40</v>
+      </c>
       <c r="E65">
         <v>1405</v>
       </c>
       <c r="F65" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" t="s">
+        <v>40</v>
+      </c>
       <c r="E66">
         <v>1409</v>
       </c>
       <c r="F66" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" t="s">
+        <v>40</v>
+      </c>
       <c r="E67">
         <v>1415</v>
       </c>
       <c r="F67" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" t="s">
+        <v>40</v>
+      </c>
       <c r="E68">
         <v>1425</v>
       </c>
       <c r="F68" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69" t="s">
+        <v>40</v>
+      </c>
       <c r="E69">
         <v>1438</v>
       </c>
       <c r="F69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" t="s">
+        <v>40</v>
+      </c>
       <c r="E70">
         <v>1485</v>
       </c>
       <c r="F70" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" t="s">
+        <v>40</v>
+      </c>
       <c r="E71">
         <v>1530</v>
       </c>
       <c r="F71" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" t="s">
+        <v>40</v>
+      </c>
       <c r="E72">
         <v>1575</v>
       </c>
       <c r="F72" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>40</v>
+      </c>
       <c r="E73">
         <v>1622</v>
       </c>
       <c r="F73" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74" t="s">
+        <v>40</v>
+      </c>
       <c r="E74">
         <v>1630</v>
       </c>
       <c r="F74" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" t="s">
+        <v>40</v>
+      </c>
       <c r="E75">
         <v>1636</v>
       </c>
       <c r="F75" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" t="s">
+        <v>40</v>
+      </c>
       <c r="E76">
         <v>1640</v>
       </c>
       <c r="F76" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77" t="s">
+        <v>40</v>
+      </c>
       <c r="E77">
         <v>1645</v>
       </c>
       <c r="F77" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" t="s">
+        <v>40</v>
+      </c>
       <c r="E78">
         <v>1656</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" t="s">
+        <v>40</v>
+      </c>
       <c r="E79">
         <v>1671</v>
       </c>
       <c r="F79" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" t="s">
+        <v>39</v>
+      </c>
+      <c r="D80" t="s">
+        <v>40</v>
+      </c>
       <c r="E80">
         <v>1718</v>
       </c>
       <c r="F80" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D81" t="s">
+        <v>40</v>
+      </c>
       <c r="E81">
         <v>1765</v>
       </c>
       <c r="F81" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" t="s">
+        <v>39</v>
+      </c>
+      <c r="D82" t="s">
+        <v>40</v>
+      </c>
       <c r="E82">
         <v>1812</v>
       </c>
       <c r="F82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" t="s">
+        <v>80</v>
+      </c>
+      <c r="E84">
+        <v>35</v>
+      </c>
+      <c r="F84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>79</v>
+      </c>
+      <c r="C85" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" t="s">
+        <v>80</v>
+      </c>
+      <c r="E85">
+        <v>38</v>
+      </c>
+      <c r="F85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" t="s">
+        <v>80</v>
+      </c>
+      <c r="E86">
+        <v>62</v>
+      </c>
+      <c r="F86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" t="s">
+        <v>80</v>
+      </c>
+      <c r="E87">
         <v>67</v>
       </c>
+      <c r="F87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88">
+        <v>89</v>
+      </c>
+      <c r="F88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89">
+        <v>97</v>
+      </c>
+      <c r="F89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>79</v>
+      </c>
+      <c r="C90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D90" t="s">
+        <v>80</v>
+      </c>
+      <c r="E90">
+        <v>102</v>
+      </c>
+      <c r="F90" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>79</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91">
+        <v>105</v>
+      </c>
+      <c r="F91" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" t="s">
+        <v>39</v>
+      </c>
+      <c r="D92" t="s">
+        <v>80</v>
+      </c>
+      <c r="E92">
+        <v>128</v>
+      </c>
+      <c r="F92" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>79</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93" t="s">
+        <v>80</v>
+      </c>
+      <c r="E93">
+        <v>130</v>
+      </c>
+      <c r="F93" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" t="s">
+        <v>80</v>
+      </c>
+      <c r="E94">
+        <v>133</v>
+      </c>
+      <c r="F94" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>79</v>
+      </c>
+      <c r="C95" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" t="s">
+        <v>80</v>
+      </c>
+      <c r="E95">
+        <v>140</v>
+      </c>
+      <c r="F95" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>79</v>
+      </c>
+      <c r="C96" t="s">
+        <v>39</v>
+      </c>
+      <c r="D96" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96">
+        <v>148</v>
+      </c>
+      <c r="F96" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>79</v>
+      </c>
+      <c r="C97" t="s">
+        <v>39</v>
+      </c>
+      <c r="D97" t="s">
+        <v>80</v>
+      </c>
+      <c r="E97">
+        <v>154</v>
+      </c>
+      <c r="F97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C98" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98" t="s">
+        <v>80</v>
+      </c>
+      <c r="E98">
+        <v>159</v>
+      </c>
+      <c r="F98" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>79</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>80</v>
+      </c>
+      <c r="E99">
+        <v>163</v>
+      </c>
+      <c r="F99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" t="s">
+        <v>80</v>
+      </c>
+      <c r="E100">
+        <v>170</v>
+      </c>
+      <c r="F100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>79</v>
+      </c>
+      <c r="C101" t="s">
+        <v>39</v>
+      </c>
+      <c r="D101" t="s">
+        <v>80</v>
+      </c>
+      <c r="E101">
+        <v>188</v>
+      </c>
+      <c r="F101" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>79</v>
+      </c>
+      <c r="C102" t="s">
+        <v>39</v>
+      </c>
+      <c r="D102" t="s">
+        <v>80</v>
+      </c>
+      <c r="E102">
+        <v>212</v>
+      </c>
+      <c r="F102" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" t="s">
+        <v>80</v>
+      </c>
+      <c r="E103">
+        <v>224</v>
+      </c>
+      <c r="F103" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" t="s">
+        <v>80</v>
+      </c>
+      <c r="E104">
+        <v>230</v>
+      </c>
+      <c r="F104" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>35</v>
+      </c>
+      <c r="B105" t="s">
+        <v>79</v>
+      </c>
+      <c r="C105" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" t="s">
+        <v>80</v>
+      </c>
+      <c r="E105">
+        <v>238</v>
+      </c>
+      <c r="F105" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>79</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+      <c r="D106" t="s">
+        <v>80</v>
+      </c>
+      <c r="E106">
+        <v>241</v>
+      </c>
+      <c r="F106" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107" t="s">
+        <v>80</v>
+      </c>
+      <c r="E107">
+        <v>248</v>
+      </c>
+      <c r="F107" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" t="s">
+        <v>79</v>
+      </c>
+      <c r="C108" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" t="s">
+        <v>80</v>
+      </c>
+      <c r="E108">
+        <v>256</v>
+      </c>
+      <c r="F108" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>35</v>
+      </c>
+      <c r="B109" t="s">
+        <v>79</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+      <c r="D109" t="s">
+        <v>80</v>
+      </c>
+      <c r="E109">
+        <v>258</v>
+      </c>
+      <c r="F109" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>79</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+      <c r="D110" t="s">
+        <v>80</v>
+      </c>
+      <c r="E110">
+        <v>264</v>
+      </c>
+      <c r="F110" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>79</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" t="s">
+        <v>80</v>
+      </c>
+      <c r="E111">
+        <v>268</v>
+      </c>
+      <c r="F111" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>35</v>
+      </c>
+      <c r="B112" t="s">
+        <v>79</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D112" t="s">
+        <v>80</v>
+      </c>
+      <c r="E112">
+        <v>272</v>
+      </c>
+      <c r="F112" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>79</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" t="s">
+        <v>80</v>
+      </c>
+      <c r="E113">
+        <v>275</v>
+      </c>
+      <c r="F113" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>79</v>
+      </c>
+      <c r="C114" t="s">
+        <v>39</v>
+      </c>
+      <c r="D114" t="s">
+        <v>80</v>
+      </c>
+      <c r="E114">
+        <v>279</v>
+      </c>
+      <c r="F114" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>79</v>
+      </c>
+      <c r="C115" t="s">
+        <v>39</v>
+      </c>
+      <c r="D115" t="s">
+        <v>80</v>
+      </c>
+      <c r="E115">
+        <v>294</v>
+      </c>
+      <c r="F115" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>79</v>
+      </c>
+      <c r="C116" t="s">
+        <v>39</v>
+      </c>
+      <c r="D116" t="s">
+        <v>80</v>
+      </c>
+      <c r="E116">
+        <v>305</v>
+      </c>
+      <c r="F116" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>113</v>
+      </c>
+      <c r="C118" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" t="s">
+        <v>40</v>
+      </c>
+      <c r="E118">
+        <v>36</v>
+      </c>
+      <c r="F118" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>35</v>
+      </c>
+      <c r="B119" t="s">
+        <v>113</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+      <c r="D119" t="s">
+        <v>40</v>
+      </c>
+      <c r="E119">
+        <v>45</v>
+      </c>
+      <c r="F119" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>113</v>
+      </c>
+      <c r="C120" t="s">
+        <v>39</v>
+      </c>
+      <c r="D120" t="s">
+        <v>40</v>
+      </c>
+      <c r="E120">
+        <v>75</v>
+      </c>
+      <c r="F120" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>113</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121" t="s">
+        <v>40</v>
+      </c>
+      <c r="E121">
+        <v>83</v>
+      </c>
+      <c r="F121" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>113</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122" t="s">
+        <v>40</v>
+      </c>
+      <c r="E122">
+        <v>92</v>
+      </c>
+      <c r="F122" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>113</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" t="s">
+        <v>40</v>
+      </c>
+      <c r="E123">
+        <v>93</v>
+      </c>
+      <c r="F123" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>113</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" t="s">
+        <v>40</v>
+      </c>
+      <c r="E124">
+        <v>102</v>
+      </c>
+      <c r="F124" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>113</v>
+      </c>
+      <c r="C125" t="s">
+        <v>39</v>
+      </c>
+      <c r="D125" t="s">
+        <v>40</v>
+      </c>
+      <c r="E125">
+        <v>110</v>
+      </c>
+      <c r="F125" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>113</v>
+      </c>
+      <c r="C126" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126" t="s">
+        <v>40</v>
+      </c>
+      <c r="E126">
+        <v>117</v>
+      </c>
+      <c r="F126" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>113</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127" t="s">
+        <v>40</v>
+      </c>
+      <c r="E127">
+        <v>124</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>113</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128" t="s">
+        <v>40</v>
+      </c>
+      <c r="E128">
+        <v>131</v>
+      </c>
+      <c r="F128" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>113</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129" t="s">
+        <v>40</v>
+      </c>
+      <c r="E129">
+        <v>138</v>
+      </c>
+      <c r="F129" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>113</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130" t="s">
+        <v>40</v>
+      </c>
+      <c r="E130">
+        <v>146</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>113</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131" t="s">
+        <v>40</v>
+      </c>
+      <c r="E131">
+        <v>153</v>
+      </c>
+      <c r="F131" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>113</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132" t="s">
+        <v>40</v>
+      </c>
+      <c r="E132">
+        <v>161</v>
+      </c>
+      <c r="F132" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>113</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133" t="s">
+        <v>40</v>
+      </c>
+      <c r="E133">
+        <v>161</v>
+      </c>
+      <c r="F133" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>130</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135" t="s">
+        <v>80</v>
+      </c>
+      <c r="E135">
+        <v>39</v>
+      </c>
+      <c r="F135" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>